<commit_message>
Continued work on Gantt chart, need to add more
</commit_message>
<xml_diff>
--- a/Gantt project chart1.xlsx
+++ b/Gantt project chart1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A264913-71A3-46CF-A829-AF03054CDE91}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B0616A10-7300-41C0-95A1-66D8E39E9DF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tracker" sheetId="4" r:id="rId1"/>
@@ -736,13 +736,13 @@
                   <c:v>43838</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43892</c:v>
+                  <c:v>43870</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43892</c:v>
+                  <c:v>43886</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43892</c:v>
+                  <c:v>43877</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>43892</c:v>
@@ -791,7 +791,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09ADD801-A7A0-4224-85D9-F08B584676CE}" type="CELLRANGE">
+                    <a:fld id="{F524B55E-3C91-48B3-8E9B-956109529D66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -824,7 +824,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E729199-490D-4EE3-B080-C444BC121897}" type="CELLRANGE">
+                    <a:fld id="{43789D3D-9E99-458B-8734-BB348B211EC3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -857,7 +857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BA76E7C-37C8-4D66-BE9A-50F1B0B77DB8}" type="CELLRANGE">
+                    <a:fld id="{1012CB4E-E4CD-4F17-94D8-2CFFCC54744B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -890,7 +890,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90BAD3B0-5C0C-4B1D-B080-439BC4271D3F}" type="CELLRANGE">
+                    <a:fld id="{485F86EB-DDFD-4602-9E42-2A14AB2B371B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -923,7 +923,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D80E019-5332-4BC9-A26D-4C8585E30304}" type="CELLRANGE">
+                    <a:fld id="{E2839C2A-1521-4B5F-9E4D-947575AC91F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1029,13 +1029,13 @@
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2194,8 +2194,8 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,54 +2315,66 @@
       <c r="B7" s="26">
         <v>2</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="11">
+        <v>43870</v>
+      </c>
+      <c r="D7" s="11">
+        <v>43892</v>
+      </c>
       <c r="E7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="27" t="str">
+      <c r="F7" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C7)-INT($C$6)),"")</f>
-        <v/>
-      </c>
-      <c r="G7" s="27" t="str">
+        <v>32</v>
+      </c>
+      <c r="G7" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v/>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="26">
         <v>3</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="C8" s="11">
+        <v>43886</v>
+      </c>
+      <c r="D8" s="11">
+        <v>43892</v>
+      </c>
       <c r="E8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="27" t="str">
+      <c r="F8" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C8)-INT($C$6)),"")</f>
-        <v/>
-      </c>
-      <c r="G8" s="27" t="str">
+        <v>48</v>
+      </c>
+      <c r="G8" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v/>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="26">
         <v>4</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="11">
+        <v>43877</v>
+      </c>
+      <c r="D9" s="11">
+        <v>43892</v>
+      </c>
       <c r="E9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="27" t="str">
+      <c r="F9" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C9)-INT($C$6)),"")</f>
-        <v/>
-      </c>
-      <c r="G9" s="27" t="str">
+        <v>39</v>
+      </c>
+      <c r="G9" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v/>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2569,7 +2581,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2774,15 +2786,15 @@
       </c>
       <c r="C7" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$C7,$B$3,0,1,1))=0,End_Date,INDEX(Milestones[],'Project Tracker'!$B7+$B$3,2)),"")</f>
-        <v>43892</v>
-      </c>
-      <c r="D7" s="9" t="str">
+        <v>43870</v>
+      </c>
+      <c r="D7" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$F7,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B7+$B$3,5)),"")</f>
-        <v/>
-      </c>
-      <c r="E7" s="17" t="str">
+        <v>32</v>
+      </c>
+      <c r="E7" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G7,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B7+$B$3,6)),"")</f>
-        <v/>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2792,15 +2804,15 @@
       </c>
       <c r="C8" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$C8,$B$3,0,1,1))=0,End_Date,INDEX(Milestones[],'Project Tracker'!$B8+$B$3,2)),"")</f>
-        <v>43892</v>
-      </c>
-      <c r="D8" s="9" t="str">
+        <v>43886</v>
+      </c>
+      <c r="D8" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$F8,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B8+$B$3,5)),"")</f>
-        <v/>
-      </c>
-      <c r="E8" s="17" t="str">
+        <v>48</v>
+      </c>
+      <c r="E8" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G8,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B8+$B$3,6)),"")</f>
-        <v/>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2811,15 +2823,15 @@
       </c>
       <c r="C9" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$C9,$B$3,0,1,1))=0,End_Date,INDEX(Milestones[],'Project Tracker'!$B9+$B$3,2)),"")</f>
-        <v>43892</v>
-      </c>
-      <c r="D9" s="9" t="str">
+        <v>43877</v>
+      </c>
+      <c r="D9" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$F9,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B9+$B$3,5)),"")</f>
-        <v/>
-      </c>
-      <c r="E9" s="17" t="str">
+        <v>39</v>
+      </c>
+      <c r="E9" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G9,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B9+$B$3,6)),"")</f>
-        <v/>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Quick fix to chart
</commit_message>
<xml_diff>
--- a/Gantt project chart1.xlsx
+++ b/Gantt project chart1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B0616A10-7300-41C0-95A1-66D8E39E9DF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{4BD552BD-0B2A-42C0-AFDB-62FCB43E8357}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tracker" sheetId="4" r:id="rId1"/>
@@ -715,13 +715,13 @@
                   <c:v>Start</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>System Testing</c:v>
+                  <c:v>Unit Testing</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Subsystem Testing</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Unit Testing</c:v>
+                  <c:v>System Testing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -791,7 +791,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F524B55E-3C91-48B3-8E9B-956109529D66}" type="CELLRANGE">
+                    <a:fld id="{0EB089D8-137B-4CA2-8CD2-1E13F982B36F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -824,7 +824,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43789D3D-9E99-458B-8734-BB348B211EC3}" type="CELLRANGE">
+                    <a:fld id="{541942FC-AF7E-4C8D-A685-B2D0C48D6FB4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -857,7 +857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1012CB4E-E4CD-4F17-94D8-2CFFCC54744B}" type="CELLRANGE">
+                    <a:fld id="{898A24F1-6EF9-482E-8845-991E91E031A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -890,7 +890,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{485F86EB-DDFD-4602-9E42-2A14AB2B371B}" type="CELLRANGE">
+                    <a:fld id="{20B8BFF9-0243-4C99-80DB-68D8552076B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -923,7 +923,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2839C2A-1521-4B5F-9E4D-947575AC91F8}" type="CELLRANGE">
+                    <a:fld id="{A6BB8C8F-162D-4790-854C-E84B84CDFEE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1008,13 +1008,13 @@
                   <c:v>Start</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>System Testing</c:v>
+                  <c:v>Unit Testing</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Subsystem Testing</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Unit Testing</c:v>
+                  <c:v>System Testing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1053,13 +1053,13 @@
                     <c:v>Start</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>System Testing</c:v>
+                    <c:v>Unit Testing</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Subsystem Testing</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Unit Testing</c:v>
+                    <c:v>System Testing</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -2194,7 +2194,7 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2322,7 +2322,7 @@
         <v>43892</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F7" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C7)-INT($C$6)),"")</f>
@@ -2366,7 +2366,7 @@
         <v>43892</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C9)-INT($C$6)),"")</f>
@@ -2581,7 +2581,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2782,7 +2782,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$E7,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B7+$B$3,4)),"")</f>
-        <v>System Testing</v>
+        <v>Unit Testing</v>
       </c>
       <c r="C7" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$C7,$B$3,0,1,1))=0,End_Date,INDEX(Milestones[],'Project Tracker'!$B7+$B$3,2)),"")</f>
@@ -2819,7 +2819,7 @@
       <c r="A9" s="22"/>
       <c r="B9" s="16" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$E9,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B9+$B$3,4)),"")</f>
-        <v>Unit Testing</v>
+        <v>System Testing</v>
       </c>
       <c r="C9" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$C9,$B$3,0,1,1))=0,End_Date,INDEX(Milestones[],'Project Tracker'!$B9+$B$3,2)),"")</f>

</xml_diff>

<commit_message>
Another quick fix to chart
</commit_message>
<xml_diff>
--- a/Gantt project chart1.xlsx
+++ b/Gantt project chart1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{4BD552BD-0B2A-42C0-AFDB-62FCB43E8357}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A69B421-D4B2-4F7F-843F-103B505407E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tracker" sheetId="4" r:id="rId1"/>
@@ -739,10 +739,10 @@
                   <c:v>43870</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43886</c:v>
+                  <c:v>43877</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43877</c:v>
+                  <c:v>43886</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>43892</c:v>
@@ -791,7 +791,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EB089D8-137B-4CA2-8CD2-1E13F982B36F}" type="CELLRANGE">
+                    <a:fld id="{14D8CFE9-2A0B-44E9-BEF5-3EFD1236C569}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -824,7 +824,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{541942FC-AF7E-4C8D-A685-B2D0C48D6FB4}" type="CELLRANGE">
+                    <a:fld id="{4EB9C7AA-E0C0-4B17-8C68-186A49F30B9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -857,7 +857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{898A24F1-6EF9-482E-8845-991E91E031A9}" type="CELLRANGE">
+                    <a:fld id="{87EE5480-1F7D-40CD-A6AB-37C07CCEC7FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -890,7 +890,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20B8BFF9-0243-4C99-80DB-68D8552076B9}" type="CELLRANGE">
+                    <a:fld id="{6AEB78E7-7E38-4300-ADBA-D5CFC3DAFB6E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -941,7 +941,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1032,10 +1031,10 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2195,7 +2194,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,7 +2337,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="11">
-        <v>43886</v>
+        <v>43877</v>
       </c>
       <c r="D8" s="11">
         <v>43892</v>
@@ -2348,11 +2347,11 @@
       </c>
       <c r="F8" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C8)-INT($C$6)),"")</f>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G8" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2360,7 +2359,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="11">
-        <v>43877</v>
+        <v>43886</v>
       </c>
       <c r="D9" s="11">
         <v>43892</v>
@@ -2370,11 +2369,11 @@
       </c>
       <c r="F9" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C9)-INT($C$6)),"")</f>
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G9" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2804,15 +2803,15 @@
       </c>
       <c r="C8" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$C8,$B$3,0,1,1))=0,End_Date,INDEX(Milestones[],'Project Tracker'!$B8+$B$3,2)),"")</f>
-        <v>43886</v>
+        <v>43877</v>
       </c>
       <c r="D8" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$F8,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B8+$B$3,5)),"")</f>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E8" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G8,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B8+$B$3,6)),"")</f>
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2823,15 +2822,15 @@
       </c>
       <c r="C9" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$C9,$B$3,0,1,1))=0,End_Date,INDEX(Milestones[],'Project Tracker'!$B9+$B$3,2)),"")</f>
-        <v>43877</v>
+        <v>43886</v>
       </c>
       <c r="D9" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$F9,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B9+$B$3,5)),"")</f>
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E9" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G9,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B9+$B$3,6)),"")</f>
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding more to chart
</commit_message>
<xml_diff>
--- a/Gantt project chart1.xlsx
+++ b/Gantt project chart1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A69B421-D4B2-4F7F-843F-103B505407E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D44884-ECE1-4E0B-8E85-310A43848CA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Start Date</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Unit Testing</t>
+  </si>
+  <si>
+    <t>Test Creation</t>
+  </si>
+  <si>
+    <t>Test Documentation</t>
   </si>
 </sst>
 </file>
@@ -710,7 +716,7 @@
             <c:strRef>
               <c:f>'Dynamic Chart Data Hidden'!$B$6:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Start</c:v>
                 </c:pt>
@@ -722,6 +728,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>System Testing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test Creation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -745,7 +754,7 @@
                   <c:v>43886</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43892</c:v>
+                  <c:v>43838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -791,7 +800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14D8CFE9-2A0B-44E9-BEF5-3EFD1236C569}" type="CELLRANGE">
+                    <a:fld id="{06878963-BCDD-4EF5-AD91-3CCFB01C200B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -824,7 +833,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4EB9C7AA-E0C0-4B17-8C68-186A49F30B9A}" type="CELLRANGE">
+                    <a:fld id="{8F88B2BE-8D15-4D0E-A96E-63E267D919F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -857,7 +866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87EE5480-1F7D-40CD-A6AB-37C07CCEC7FE}" type="CELLRANGE">
+                    <a:fld id="{A5FBBD1A-D027-40DD-B302-072B74B07F31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -890,7 +899,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AEB78E7-7E38-4300-ADBA-D5CFC3DAFB6E}" type="CELLRANGE">
+                    <a:fld id="{B780BA5C-BFD7-4DBB-BD04-00449BBEC3F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -923,7 +932,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6BB8C8F-162D-4790-854C-E84B84CDFEE9}" type="CELLRANGE">
+                    <a:fld id="{6CD2CB79-A52E-4CB2-B74A-CB63431AD54D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -941,6 +950,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1002,7 +1012,7 @@
             <c:strRef>
               <c:f>'Dynamic Chart Data Hidden'!$B$6:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Start</c:v>
                 </c:pt>
@@ -1015,6 +1025,9 @@
                 <c:pt idx="3">
                   <c:v>System Testing</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test Creation</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
@@ -1025,19 +1038,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1059,6 +1072,9 @@
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>System Testing</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Test Creation</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -2194,7 +2210,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2238,7 +2254,7 @@
       </c>
       <c r="D3" s="18">
         <f ca="1">IFERROR(IF(MAX(Milestones[End Date])=0,TODAY(),MAX(Milestones[End Date])),TODAY())</f>
-        <v>43892</v>
+        <v>43939</v>
       </c>
       <c r="E3" s="20"/>
     </row>
@@ -2296,7 +2312,7 @@
         <v>43838</v>
       </c>
       <c r="D6" s="11">
-        <v>43892</v>
+        <v>43939</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
@@ -2307,7 +2323,7 @@
       </c>
       <c r="G6" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v>55</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2318,7 +2334,7 @@
         <v>43870</v>
       </c>
       <c r="D7" s="11">
-        <v>43892</v>
+        <v>43939</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>44</v>
@@ -2329,7 +2345,7 @@
       </c>
       <c r="G7" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2340,7 +2356,7 @@
         <v>43877</v>
       </c>
       <c r="D8" s="11">
-        <v>43892</v>
+        <v>43939</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>43</v>
@@ -2351,7 +2367,7 @@
       </c>
       <c r="G8" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v>16</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2362,7 +2378,7 @@
         <v>43886</v>
       </c>
       <c r="D9" s="11">
-        <v>43892</v>
+        <v>43939</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>42</v>
@@ -2373,35 +2389,51 @@
       </c>
       <c r="G9" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="27" t="str">
+      <c r="B10" s="26">
+        <v>5</v>
+      </c>
+      <c r="C10" s="11">
+        <v>43838</v>
+      </c>
+      <c r="D10" s="11">
+        <v>43939</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C10)-INT($C$6)),"")</f>
-        <v/>
-      </c>
-      <c r="G10" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="G10" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v/>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="27" t="str">
+      <c r="B11" s="26">
+        <v>6</v>
+      </c>
+      <c r="C11" s="11">
+        <v>43892</v>
+      </c>
+      <c r="D11" s="11">
+        <v>43939</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="27">
         <f>IFERROR(IF(OR(LEN(Milestones[[#This Row],[Start Date]])=0,LEN(Milestones[[#This Row],[End Date]])=0),"",INT(C11)-INT($C$6)),"")</f>
-        <v/>
-      </c>
-      <c r="G11" s="27" t="str">
+        <v>54</v>
+      </c>
+      <c r="G11" s="27">
         <f>IFERROR(IF(Milestones[[#This Row],[Start on Day]]=0,DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1,IF(LEN(Milestones[[#This Row],[Start on Day]])=0,"",DATEDIF(Milestones[[#This Row],[Start Date]],Milestones[[#This Row],[End Date]],"d")+1)),0)</f>
-        <v/>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2775,7 +2807,7 @@
       </c>
       <c r="E6" s="15">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G6,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B6+$B$3,6)),"")</f>
-        <v>55</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2793,7 +2825,7 @@
       </c>
       <c r="E7" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G7,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B7+$B$3,6)),"")</f>
-        <v>23</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2811,7 +2843,7 @@
       </c>
       <c r="E8" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G8,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B8+$B$3,6)),"")</f>
-        <v>16</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2830,26 +2862,26 @@
       </c>
       <c r="E9" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G9,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B9+$B$3,6)),"")</f>
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="16" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$E10,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B10+$B$3,4)),"")</f>
-        <v/>
+        <v>Test Creation</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$C10,$B$3,0,1,1))=0,End_Date,INDEX(Milestones[],'Project Tracker'!$B10+$B$3,2)),"")</f>
-        <v>43892</v>
-      </c>
-      <c r="D10" s="9" t="str">
+        <v>43838</v>
+      </c>
+      <c r="D10" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$F10,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B10+$B$3,5)),"")</f>
-        <v/>
-      </c>
-      <c r="E10" s="17" t="str">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Project Tracker'!$G10,$B$3,0,1,1))=0,"",INDEX(Milestones[],'Project Tracker'!$B10+$B$3,6)),"")</f>
-        <v/>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>